<commit_message>
ready for take off
</commit_message>
<xml_diff>
--- a/inv_adv_human_labels.xlsx
+++ b/inv_adv_human_labels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bachelorarbeit\Code\bachelorthesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bachelorarbeit\Code\bachelorthesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A36CD7B-6775-4A31-ABF8-C069A7F8727B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEFB2DB-64A1-4164-BEED-164A02BC3592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2592"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="A457" workbookViewId="0">
+      <selection activeCell="N493" sqref="N493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +622,7 @@
         <v>7</v>
       </c>
       <c r="K3" s="8">
-        <f>MODE(A3:J3)</f>
+        <f t="shared" ref="K3:K66" si="0">MODE(A3:J3)</f>
         <v>7</v>
       </c>
       <c r="L3" s="10">
@@ -661,7 +661,7 @@
         <v>2</v>
       </c>
       <c r="K4" s="8">
-        <f>MODE(A4:J4)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L4" s="10">
@@ -700,7 +700,7 @@
         <v>1</v>
       </c>
       <c r="K5" s="8">
-        <f>MODE(A5:J5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5" s="8">
@@ -739,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="8">
-        <f>MODE(A6:J6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L6" s="8">
@@ -778,7 +778,7 @@
         <v>9</v>
       </c>
       <c r="K7" s="8">
-        <f>MODE(A7:J7)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L7" s="11">
@@ -817,7 +817,7 @@
         <v>7</v>
       </c>
       <c r="K8" s="8">
-        <f>MODE(A8:J8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8" s="11">
@@ -856,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="K9" s="8">
-        <f>MODE(A9:J9)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L9" s="11">
@@ -895,7 +895,7 @@
         <v>9</v>
       </c>
       <c r="K10" s="8">
-        <f>MODE(A10:J10)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L10" s="11">
@@ -934,7 +934,7 @@
         <v>8</v>
       </c>
       <c r="K11" s="8">
-        <f>MODE(A11:J11)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L11" s="11">
@@ -973,7 +973,7 @@
         <v>9</v>
       </c>
       <c r="K12" s="8">
-        <f>MODE(A12:J12)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L12" s="11">
@@ -1012,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="8">
-        <f>MODE(A13:J13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L13" s="11">
@@ -1051,7 +1051,7 @@
         <v>6</v>
       </c>
       <c r="K14" s="8">
-        <f>MODE(A14:J14)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L14" s="11">
@@ -1090,7 +1090,7 @@
         <v>9</v>
       </c>
       <c r="K15" s="8">
-        <f>MODE(A15:J15)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L15" s="11">
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="8">
-        <f>MODE(A16:J16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L16" s="11">
@@ -1168,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="8">
-        <f>MODE(A17:J17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L17" s="11">
@@ -1207,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="K18" s="8">
-        <f>MODE(A18:J18)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L18" s="11">
@@ -1246,7 +1246,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="8">
-        <f>MODE(A19:J19)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L19" s="11">
@@ -1285,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="K20" s="8">
-        <f>MODE(A20:J20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L20" s="11">
@@ -1324,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="K21" s="8">
-        <f>MODE(A21:J21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L21" s="11">
@@ -1363,7 +1363,7 @@
         <v>4</v>
       </c>
       <c r="K22" s="8">
-        <f>MODE(A22:J22)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L22" s="11">
@@ -1402,7 +1402,7 @@
         <v>9</v>
       </c>
       <c r="K23" s="8">
-        <f>MODE(A23:J23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L23" s="11">
@@ -1441,7 +1441,7 @@
         <v>6</v>
       </c>
       <c r="K24" s="8">
-        <f>MODE(A24:J24)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L24" s="11">
@@ -1480,7 +1480,7 @@
         <v>6</v>
       </c>
       <c r="K25" s="8">
-        <f>MODE(A25:J25)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L25" s="11">
@@ -1519,7 +1519,7 @@
         <v>5</v>
       </c>
       <c r="K26" s="8">
-        <f>MODE(A26:J26)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L26" s="11">
@@ -1558,7 +1558,7 @@
         <v>4</v>
       </c>
       <c r="K27" s="8">
-        <f>MODE(A27:J27)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L27" s="11">
@@ -1597,7 +1597,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="8">
-        <f>MODE(A28:J28)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L28" s="11">
@@ -1636,7 +1636,7 @@
         <v>7</v>
       </c>
       <c r="K29" s="8">
-        <f>MODE(A29:J29)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L29" s="11">
@@ -1675,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="8">
-        <f>MODE(A30:J30)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L30" s="11">
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="8">
-        <f>MODE(A31:J31)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L31" s="11">
@@ -1753,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="8">
-        <f>MODE(A32:J32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L32" s="11">
@@ -1792,7 +1792,7 @@
         <v>3</v>
       </c>
       <c r="K33" s="8">
-        <f>MODE(A33:J33)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L33" s="11">
@@ -1831,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="8">
-        <f>MODE(A34:J34)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L34" s="11">
@@ -1870,7 +1870,7 @@
         <v>3</v>
       </c>
       <c r="K35" s="8">
-        <f>MODE(A35:J35)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L35" s="11">
@@ -1909,7 +1909,7 @@
         <v>4</v>
       </c>
       <c r="K36" s="8">
-        <f>MODE(A36:J36)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L36" s="11">
@@ -1948,7 +1948,7 @@
         <v>7</v>
       </c>
       <c r="K37" s="8">
-        <f>MODE(A37:J37)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L37" s="11">
@@ -1987,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="K38" s="8">
-        <f>MODE(A38:J38)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L38" s="11">
@@ -2026,7 +2026,7 @@
         <v>2</v>
       </c>
       <c r="K39" s="8">
-        <f>MODE(A39:J39)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L39" s="11">
@@ -2065,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="8">
-        <f>MODE(A40:J40)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L40" s="11">
@@ -2104,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="K41" s="8">
-        <f>MODE(A41:J41)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L41" s="11">
@@ -2143,7 +2143,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="8">
-        <f>MODE(A42:J42)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L42" s="11">
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
       <c r="K43" s="8">
-        <f>MODE(A43:J43)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L43" s="11">
@@ -2221,7 +2221,7 @@
         <v>7</v>
       </c>
       <c r="K44" s="8">
-        <f>MODE(A44:J44)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L44" s="11">
@@ -2260,7 +2260,7 @@
         <v>4</v>
       </c>
       <c r="K45" s="8">
-        <f>MODE(A45:J45)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L45" s="11">
@@ -2299,7 +2299,7 @@
         <v>2</v>
       </c>
       <c r="K46" s="8">
-        <f>MODE(A46:J46)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L46" s="11">
@@ -2338,7 +2338,7 @@
         <v>8</v>
       </c>
       <c r="K47" s="8">
-        <f>MODE(A47:J47)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L47" s="11">
@@ -2377,7 +2377,7 @@
         <v>5</v>
       </c>
       <c r="K48" s="8">
-        <f>MODE(A48:J48)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L48" s="11">
@@ -2416,7 +2416,7 @@
         <v>1</v>
       </c>
       <c r="K49" s="8">
-        <f>MODE(A49:J49)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L49" s="11">
@@ -2455,7 +2455,7 @@
         <v>2</v>
       </c>
       <c r="K50" s="8">
-        <f>MODE(A50:J50)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L50" s="11">
@@ -2494,7 +2494,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="8">
-        <f>MODE(A51:J51)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L51" s="11">
@@ -2533,7 +2533,7 @@
         <v>4</v>
       </c>
       <c r="K52" s="8">
-        <f>MODE(A52:J52)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L52" s="11">
@@ -2572,7 +2572,7 @@
         <v>6</v>
       </c>
       <c r="K53" s="8">
-        <f>MODE(A53:J53)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L53" s="11">
@@ -2612,7 +2612,7 @@
         <v>8</v>
       </c>
       <c r="K54" s="8">
-        <f>MODE(A54:J54)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L54" s="11">
@@ -2651,7 +2651,7 @@
         <v>5</v>
       </c>
       <c r="K55" s="8">
-        <f>MODE(A55:J55)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L55" s="11">
@@ -2690,7 +2690,7 @@
         <v>5</v>
       </c>
       <c r="K56" s="8">
-        <f>MODE(A56:J56)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L56" s="11">
@@ -2729,7 +2729,7 @@
         <v>6</v>
       </c>
       <c r="K57" s="8">
-        <f>MODE(A57:J57)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L57" s="11">
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="8">
-        <f>MODE(A58:J58)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L58" s="11">
@@ -2807,7 +2807,7 @@
         <v>4</v>
       </c>
       <c r="K59" s="8">
-        <f>MODE(A59:J59)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L59" s="11">
@@ -2846,7 +2846,7 @@
         <v>7</v>
       </c>
       <c r="K60" s="8">
-        <f>MODE(A60:J60)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L60" s="11">
@@ -2885,7 +2885,7 @@
         <v>9</v>
       </c>
       <c r="K61" s="8">
-        <f>MODE(A61:J61)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L61" s="11">
@@ -2924,7 +2924,7 @@
         <v>5</v>
       </c>
       <c r="K62" s="8">
-        <f>MODE(A62:J62)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="L62" s="11">
@@ -2963,7 +2963,7 @@
         <v>7</v>
       </c>
       <c r="K63" s="8">
-        <f>MODE(A63:J63)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L63" s="11">
@@ -3002,7 +3002,7 @@
         <v>8</v>
       </c>
       <c r="K64" s="8">
-        <f>MODE(A64:J64)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="L64" s="11">
@@ -3041,7 +3041,7 @@
         <v>9</v>
       </c>
       <c r="K65" s="8">
-        <f>MODE(A65:J65)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L65" s="11">
@@ -3080,7 +3080,7 @@
         <v>8</v>
       </c>
       <c r="K66" s="8">
-        <f>MODE(A66:J66)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L66" s="11">
@@ -3119,7 +3119,7 @@
         <v>7</v>
       </c>
       <c r="K67" s="8">
-        <f>MODE(A67:J67)</f>
+        <f t="shared" ref="K67:K130" si="1">MODE(A67:J67)</f>
         <v>7</v>
       </c>
       <c r="L67" s="11">
@@ -3158,7 +3158,7 @@
         <v>4</v>
       </c>
       <c r="K68" s="8">
-        <f>MODE(A68:J68)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L68" s="11">
@@ -3197,7 +3197,7 @@
         <v>6</v>
       </c>
       <c r="K69" s="8">
-        <f>MODE(A69:J69)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L69" s="11">
@@ -3236,7 +3236,7 @@
         <v>4</v>
       </c>
       <c r="K70" s="8">
-        <f>MODE(A70:J70)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L70" s="11">
@@ -3275,7 +3275,7 @@
         <v>3</v>
       </c>
       <c r="K71" s="8">
-        <f>MODE(A71:J71)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L71" s="11">
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="K72" s="8">
-        <f>MODE(A72:J72)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L72" s="11">
@@ -3353,7 +3353,7 @@
         <v>7</v>
       </c>
       <c r="K73" s="8">
-        <f>MODE(A73:J73)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L73" s="11">
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="K74" s="8">
-        <f>MODE(A74:J74)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L74" s="11">
@@ -3431,7 +3431,7 @@
         <v>2</v>
       </c>
       <c r="K75" s="8">
-        <f>MODE(A75:J75)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L75" s="11">
@@ -3470,7 +3470,7 @@
         <v>9</v>
       </c>
       <c r="K76" s="8">
-        <f>MODE(A76:J76)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L76" s="11">
@@ -3509,7 +3509,7 @@
         <v>1</v>
       </c>
       <c r="K77" s="8">
-        <f>MODE(A77:J77)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L77" s="11">
@@ -3548,7 +3548,7 @@
         <v>7</v>
       </c>
       <c r="K78" s="8">
-        <f>MODE(A78:J78)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L78" s="11">
@@ -3587,7 +3587,7 @@
         <v>3</v>
       </c>
       <c r="K79" s="8">
-        <f>MODE(A79:J79)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L79" s="11">
@@ -3626,7 +3626,7 @@
         <v>2</v>
       </c>
       <c r="K80" s="8">
-        <f>MODE(A80:J80)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L80" s="11">
@@ -3665,7 +3665,7 @@
         <v>9</v>
       </c>
       <c r="K81" s="8">
-        <f>MODE(A81:J81)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L81" s="11">
@@ -3704,7 +3704,7 @@
         <v>7</v>
       </c>
       <c r="K82" s="8">
-        <f>MODE(A82:J82)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L82" s="11">
@@ -3743,7 +3743,7 @@
         <v>7</v>
       </c>
       <c r="K83" s="8">
-        <f>MODE(A83:J83)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L83" s="11">
@@ -3782,7 +3782,7 @@
         <v>6</v>
       </c>
       <c r="K84" s="8">
-        <f>MODE(A84:J84)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L84" s="11">
@@ -3821,7 +3821,7 @@
         <v>2</v>
       </c>
       <c r="K85" s="8">
-        <f>MODE(A85:J85)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L85" s="11">
@@ -3860,7 +3860,7 @@
         <v>7</v>
       </c>
       <c r="K86" s="8">
-        <f>MODE(A86:J86)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L86" s="11">
@@ -3899,7 +3899,7 @@
         <v>8</v>
       </c>
       <c r="K87" s="8">
-        <f>MODE(A87:J87)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L87" s="11">
@@ -3938,7 +3938,7 @@
         <v>4</v>
       </c>
       <c r="K88" s="8">
-        <f>MODE(A88:J88)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L88" s="11">
@@ -3977,7 +3977,7 @@
         <v>7</v>
       </c>
       <c r="K89" s="8">
-        <f>MODE(A89:J89)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L89" s="11">
@@ -4016,7 +4016,7 @@
         <v>3</v>
       </c>
       <c r="K90" s="8">
-        <f>MODE(A90:J90)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L90" s="11">
@@ -4055,7 +4055,7 @@
         <v>6</v>
       </c>
       <c r="K91" s="8">
-        <f>MODE(A91:J91)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L91" s="11">
@@ -4094,7 +4094,7 @@
         <v>1</v>
       </c>
       <c r="K92" s="8">
-        <f>MODE(A92:J92)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L92" s="11">
@@ -4133,7 +4133,7 @@
         <v>8</v>
       </c>
       <c r="K93" s="8">
-        <f>MODE(A93:J93)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L93" s="11">
@@ -4172,7 +4172,7 @@
         <v>6</v>
       </c>
       <c r="K94" s="8">
-        <f>MODE(A94:J94)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L94" s="11">
@@ -4211,7 +4211,7 @@
         <v>9</v>
       </c>
       <c r="K95" s="8">
-        <f>MODE(A95:J95)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L95" s="11">
@@ -4250,7 +4250,7 @@
         <v>3</v>
       </c>
       <c r="K96" s="8">
-        <f>MODE(A96:J96)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L96" s="11">
@@ -4289,7 +4289,7 @@
         <v>1</v>
       </c>
       <c r="K97" s="8">
-        <f>MODE(A97:J97)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L97" s="11">
@@ -4328,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="K98" s="8">
-        <f>MODE(A98:J98)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L98" s="11">
@@ -4367,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="K99" s="8">
-        <f>MODE(A99:J99)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L99" s="11">
@@ -4406,7 +4406,7 @@
         <v>7</v>
       </c>
       <c r="K100" s="8">
-        <f>MODE(A100:J100)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L100" s="11">
@@ -4445,7 +4445,7 @@
         <v>6</v>
       </c>
       <c r="K101" s="8">
-        <f>MODE(A101:J101)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L101" s="11">
@@ -4484,7 +4484,7 @@
         <v>9</v>
       </c>
       <c r="K102" s="8">
-        <f>MODE(A102:J102)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L102" s="11">
@@ -4523,7 +4523,7 @@
         <v>6</v>
       </c>
       <c r="K103" s="8">
-        <f>MODE(A103:J103)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L103" s="11">
@@ -4562,7 +4562,7 @@
         <v>0</v>
       </c>
       <c r="K104" s="8">
-        <f>MODE(A104:J104)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L104" s="11">
@@ -4601,7 +4601,7 @@
         <v>5</v>
       </c>
       <c r="K105" s="8">
-        <f>MODE(A105:J105)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L105" s="11">
@@ -4640,7 +4640,7 @@
         <v>4</v>
       </c>
       <c r="K106" s="8">
-        <f>MODE(A106:J106)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L106" s="11">
@@ -4679,7 +4679,7 @@
         <v>9</v>
       </c>
       <c r="K107" s="8">
-        <f>MODE(A107:J107)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L107" s="11">
@@ -4718,7 +4718,7 @@
         <v>9</v>
       </c>
       <c r="K108" s="8">
-        <f>MODE(A108:J108)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L108" s="11">
@@ -4757,7 +4757,7 @@
         <v>2</v>
       </c>
       <c r="K109" s="8">
-        <f>MODE(A109:J109)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L109" s="11">
@@ -4796,7 +4796,7 @@
         <v>6</v>
       </c>
       <c r="K110" s="8">
-        <f>MODE(A110:J110)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L110" s="11">
@@ -4835,7 +4835,7 @@
         <v>9</v>
       </c>
       <c r="K111" s="8">
-        <f>MODE(A111:J111)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L111" s="11">
@@ -4874,7 +4874,7 @@
         <v>4</v>
       </c>
       <c r="K112" s="8">
-        <f>MODE(A112:J112)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L112" s="11">
@@ -4913,7 +4913,7 @@
         <v>8</v>
       </c>
       <c r="K113" s="8">
-        <f>MODE(A113:J113)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="L113" s="11">
@@ -4952,7 +4952,7 @@
         <v>2</v>
       </c>
       <c r="K114" s="8">
-        <f>MODE(A114:J114)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L114" s="11">
@@ -4991,7 +4991,7 @@
         <v>3</v>
       </c>
       <c r="K115" s="8">
-        <f>MODE(A115:J115)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L115" s="11">
@@ -5030,7 +5030,7 @@
         <v>9</v>
       </c>
       <c r="K116" s="8">
-        <f>MODE(A116:J116)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L116" s="11">
@@ -5069,7 +5069,7 @@
         <v>7</v>
       </c>
       <c r="K117" s="8">
-        <f>MODE(A117:J117)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L117" s="11">
@@ -5108,7 +5108,7 @@
         <v>4</v>
       </c>
       <c r="K118" s="8">
-        <f>MODE(A118:J118)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L118" s="11">
@@ -5147,7 +5147,7 @@
         <v>4</v>
       </c>
       <c r="K119" s="8">
-        <f>MODE(A119:J119)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L119" s="11">
@@ -5186,7 +5186,7 @@
         <v>4</v>
       </c>
       <c r="K120" s="8">
-        <f>MODE(A120:J120)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L120" s="11">
@@ -5225,7 +5225,7 @@
         <v>9</v>
       </c>
       <c r="K121" s="8">
-        <f>MODE(A121:J121)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L121" s="11">
@@ -5264,7 +5264,7 @@
         <v>2</v>
       </c>
       <c r="K122" s="8">
-        <f>MODE(A122:J122)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L122" s="11">
@@ -5303,7 +5303,7 @@
         <v>5</v>
       </c>
       <c r="K123" s="8">
-        <f>MODE(A123:J123)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L123" s="16">
@@ -5342,7 +5342,7 @@
         <v>9</v>
       </c>
       <c r="K124" s="8">
-        <f>MODE(A124:J124)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L124" s="16">
@@ -5381,7 +5381,7 @@
         <v>7</v>
       </c>
       <c r="K125" s="8">
-        <f>MODE(A125:J125)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L125" s="16">
@@ -5420,7 +5420,7 @@
         <v>6</v>
       </c>
       <c r="K126" s="8">
-        <f>MODE(A126:J126)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="L126" s="16">
@@ -5459,7 +5459,7 @@
         <v>7</v>
       </c>
       <c r="K127" s="8">
-        <f>MODE(A127:J127)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L127" s="16">
@@ -5498,7 +5498,7 @@
         <v>4</v>
       </c>
       <c r="K128" s="8">
-        <f>MODE(A128:J128)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="L128" s="16">
@@ -5537,7 +5537,7 @@
         <v>0</v>
       </c>
       <c r="K129" s="8">
-        <f>MODE(A129:J129)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L129" s="16">
@@ -5576,7 +5576,7 @@
         <v>5</v>
       </c>
       <c r="K130" s="8">
-        <f>MODE(A130:J130)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="L130" s="16">
@@ -5615,7 +5615,7 @@
         <v>8</v>
       </c>
       <c r="K131" s="8">
-        <f>MODE(A131:J131)</f>
+        <f t="shared" ref="K131:K194" si="2">MODE(A131:J131)</f>
         <v>8</v>
       </c>
       <c r="L131" s="16">
@@ -5654,7 +5654,7 @@
         <v>5</v>
       </c>
       <c r="K132" s="8">
-        <f>MODE(A132:J132)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L132" s="16">
@@ -5693,7 +5693,7 @@
         <v>6</v>
       </c>
       <c r="K133" s="8">
-        <f>MODE(A133:J133)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L133" s="16">
@@ -5732,7 +5732,7 @@
         <v>6</v>
       </c>
       <c r="K134" s="8">
-        <f>MODE(A134:J134)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L134" s="16">
@@ -5771,7 +5771,7 @@
         <v>5</v>
       </c>
       <c r="K135" s="8">
-        <f>MODE(A135:J135)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L135" s="16">
@@ -5810,7 +5810,7 @@
         <v>7</v>
       </c>
       <c r="K136" s="8">
-        <f>MODE(A136:J136)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L136" s="16">
@@ -5849,7 +5849,7 @@
         <v>8</v>
       </c>
       <c r="K137" s="8">
-        <f>MODE(A137:J137)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L137" s="16">
@@ -5888,7 +5888,7 @@
         <v>1</v>
       </c>
       <c r="K138" s="8">
-        <f>MODE(A138:J138)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L138" s="16">
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="K139" s="8">
-        <f>MODE(A139:J139)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L139" s="16">
@@ -5966,7 +5966,7 @@
         <v>1</v>
       </c>
       <c r="K140" s="8">
-        <f>MODE(A140:J140)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L140" s="16">
@@ -6005,7 +6005,7 @@
         <v>6</v>
       </c>
       <c r="K141" s="8">
-        <f>MODE(A141:J141)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L141" s="16">
@@ -6044,7 +6044,7 @@
         <v>9</v>
       </c>
       <c r="K142" s="8">
-        <f>MODE(A142:J142)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L142" s="16">
@@ -6083,7 +6083,7 @@
         <v>6</v>
       </c>
       <c r="K143" s="8">
-        <f>MODE(A143:J143)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L143" s="16">
@@ -6122,7 +6122,7 @@
         <v>7</v>
       </c>
       <c r="K144" s="8">
-        <f>MODE(A144:J144)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L144" s="16">
@@ -6161,7 +6161,7 @@
         <v>3</v>
       </c>
       <c r="K145" s="8">
-        <f>MODE(A145:J145)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L145" s="16">
@@ -6200,7 +6200,7 @@
         <v>1</v>
       </c>
       <c r="K146" s="8">
-        <f>MODE(A146:J146)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L146" s="16">
@@ -6239,7 +6239,7 @@
         <v>7</v>
       </c>
       <c r="K147" s="8">
-        <f>MODE(A147:J147)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L147" s="16">
@@ -6278,7 +6278,7 @@
         <v>1</v>
       </c>
       <c r="K148" s="8">
-        <f>MODE(A148:J148)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L148" s="16">
@@ -6317,7 +6317,7 @@
         <v>8</v>
       </c>
       <c r="K149" s="8">
-        <f>MODE(A149:J149)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L149" s="16">
@@ -6356,7 +6356,7 @@
         <v>2</v>
       </c>
       <c r="K150" s="8">
-        <f>MODE(A150:J150)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L150" s="16">
@@ -6395,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="K151" s="8">
-        <f>MODE(A151:J151)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L151" s="16">
@@ -6434,7 +6434,7 @@
         <v>2</v>
       </c>
       <c r="K152" s="8">
-        <f>MODE(A152:J152)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L152" s="16">
@@ -6473,7 +6473,7 @@
         <v>9</v>
       </c>
       <c r="K153" s="8">
-        <f>MODE(A153:J153)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L153" s="16">
@@ -6512,7 +6512,7 @@
         <v>9</v>
       </c>
       <c r="K154" s="8">
-        <f>MODE(A154:J154)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L154" s="16">
@@ -6551,7 +6551,7 @@
         <v>5</v>
       </c>
       <c r="K155" s="8">
-        <f>MODE(A155:J155)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L155" s="16">
@@ -6590,7 +6590,7 @@
         <v>5</v>
       </c>
       <c r="K156" s="8">
-        <f>MODE(A156:J156)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L156" s="16">
@@ -6629,7 +6629,7 @@
         <v>1</v>
       </c>
       <c r="K157" s="8">
-        <f>MODE(A157:J157)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L157" s="16">
@@ -6668,7 +6668,7 @@
         <v>5</v>
       </c>
       <c r="K158" s="8">
-        <f>MODE(A158:J158)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L158" s="16">
@@ -6707,7 +6707,7 @@
         <v>6</v>
       </c>
       <c r="K159" s="8">
-        <f>MODE(A159:J159)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L159" s="16">
@@ -6746,7 +6746,7 @@
         <v>0</v>
       </c>
       <c r="K160" s="8">
-        <f>MODE(A160:J160)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L160" s="16">
@@ -6785,7 +6785,7 @@
         <v>3</v>
       </c>
       <c r="K161" s="8">
-        <f>MODE(A161:J161)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L161" s="16">
@@ -6824,7 +6824,7 @@
         <v>4</v>
       </c>
       <c r="K162" s="8">
-        <f>MODE(A162:J162)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L162" s="16">
@@ -6863,7 +6863,7 @@
         <v>4</v>
       </c>
       <c r="K163" s="8">
-        <f>MODE(A163:J163)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L163" s="16">
@@ -6902,7 +6902,7 @@
         <v>6</v>
       </c>
       <c r="K164" s="8">
-        <f>MODE(A164:J164)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L164" s="16">
@@ -6941,7 +6941,7 @@
         <v>5</v>
       </c>
       <c r="K165" s="8">
-        <f>MODE(A165:J165)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L165" s="16">
@@ -6980,7 +6980,7 @@
         <v>4</v>
       </c>
       <c r="K166" s="8">
-        <f>MODE(A166:J166)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L166" s="16">
@@ -7019,7 +7019,7 @@
         <v>6</v>
       </c>
       <c r="K167" s="8">
-        <f>MODE(A167:J167)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="L167" s="16">
@@ -7058,7 +7058,7 @@
         <v>5</v>
       </c>
       <c r="K168" s="8">
-        <f>MODE(A168:J168)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L168" s="16">
@@ -7097,7 +7097,7 @@
         <v>4</v>
       </c>
       <c r="K169" s="8">
-        <f>MODE(A169:J169)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L169" s="16">
@@ -7136,7 +7136,7 @@
         <v>5</v>
       </c>
       <c r="K170" s="8">
-        <f>MODE(A170:J170)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L170" s="16">
@@ -7175,7 +7175,7 @@
         <v>1</v>
       </c>
       <c r="K171" s="8">
-        <f>MODE(A171:J171)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L171" s="16">
@@ -7214,7 +7214,7 @@
         <v>4</v>
       </c>
       <c r="K172" s="8">
-        <f>MODE(A172:J172)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L172" s="16">
@@ -7253,7 +7253,7 @@
         <v>9</v>
       </c>
       <c r="K173" s="8">
-        <f>MODE(A173:J173)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L173" s="16">
@@ -7292,7 +7292,7 @@
         <v>7</v>
       </c>
       <c r="K174" s="8">
-        <f>MODE(A174:J174)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L174" s="16">
@@ -7331,7 +7331,7 @@
         <v>2</v>
       </c>
       <c r="K175" s="8">
-        <f>MODE(A175:J175)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L175" s="16">
@@ -7370,7 +7370,7 @@
         <v>8</v>
       </c>
       <c r="K176" s="8">
-        <f>MODE(A176:J176)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L176" s="16">
@@ -7409,7 +7409,7 @@
         <v>2</v>
       </c>
       <c r="K177" s="8">
-        <f>MODE(A177:J177)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L177" s="16">
@@ -7448,7 +7448,7 @@
         <v>7</v>
       </c>
       <c r="K178" s="8">
-        <f>MODE(A178:J178)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="L178" s="16">
@@ -7487,7 +7487,7 @@
         <v>7</v>
       </c>
       <c r="K179" s="8">
-        <f>MODE(A179:J179)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L179" s="16">
@@ -7526,7 +7526,7 @@
         <v>8</v>
       </c>
       <c r="K180" s="8">
-        <f>MODE(A180:J180)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L180" s="16">
@@ -7565,7 +7565,7 @@
         <v>1</v>
       </c>
       <c r="K181" s="8">
-        <f>MODE(A181:J181)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L181" s="16">
@@ -7604,7 +7604,7 @@
         <v>8</v>
       </c>
       <c r="K182" s="8">
-        <f>MODE(A182:J182)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L182" s="16">
@@ -7643,7 +7643,7 @@
         <v>1</v>
       </c>
       <c r="K183" s="8">
-        <f>MODE(A183:J183)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L183" s="16">
@@ -7682,7 +7682,7 @@
         <v>8</v>
       </c>
       <c r="K184" s="8">
-        <f>MODE(A184:J184)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L184" s="16">
@@ -7721,7 +7721,7 @@
         <v>5</v>
       </c>
       <c r="K185" s="8">
-        <f>MODE(A185:J185)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L185" s="16">
@@ -7760,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="K186" s="8">
-        <f>MODE(A186:J186)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L186" s="16">
@@ -7799,7 +7799,7 @@
         <v>8</v>
       </c>
       <c r="K187" s="8">
-        <f>MODE(A187:J187)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L187" s="16">
@@ -7838,7 +7838,7 @@
         <v>9</v>
       </c>
       <c r="K188" s="8">
-        <f>MODE(A188:J188)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="L188" s="16">
@@ -7877,7 +7877,7 @@
         <v>2</v>
       </c>
       <c r="K189" s="8">
-        <f>MODE(A189:J189)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L189" s="16">
@@ -7916,7 +7916,7 @@
         <v>5</v>
       </c>
       <c r="K190" s="8">
-        <f>MODE(A190:J190)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="L190" s="16">
@@ -7955,7 +7955,7 @@
         <v>0</v>
       </c>
       <c r="K191" s="8">
-        <f>MODE(A191:J191)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L191" s="16">
@@ -7994,7 +7994,7 @@
         <v>1</v>
       </c>
       <c r="K192" s="8">
-        <f>MODE(A192:J192)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L192" s="16">
@@ -8033,7 +8033,7 @@
         <v>1</v>
       </c>
       <c r="K193" s="8">
-        <f>MODE(A193:J193)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L193" s="16">
@@ -8072,7 +8072,7 @@
         <v>1</v>
       </c>
       <c r="K194" s="8">
-        <f>MODE(A194:J194)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="L194" s="16">
@@ -8111,7 +8111,7 @@
         <v>0</v>
       </c>
       <c r="K195" s="8">
-        <f>MODE(A195:J195)</f>
+        <f t="shared" ref="K195:K258" si="3">MODE(A195:J195)</f>
         <v>0</v>
       </c>
       <c r="L195" s="16">
@@ -8150,7 +8150,7 @@
         <v>8</v>
       </c>
       <c r="K196" s="8">
-        <f>MODE(A196:J196)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L196" s="16">
@@ -8189,7 +8189,7 @@
         <v>0</v>
       </c>
       <c r="K197" s="8">
-        <f>MODE(A197:J197)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L197" s="16">
@@ -8228,7 +8228,7 @@
         <v>3</v>
       </c>
       <c r="K198" s="8">
-        <f>MODE(A198:J198)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L198" s="16">
@@ -8267,7 +8267,7 @@
         <v>1</v>
       </c>
       <c r="K199" s="8">
-        <f>MODE(A199:J199)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L199" s="16">
@@ -8306,7 +8306,7 @@
         <v>6</v>
       </c>
       <c r="K200" s="8">
-        <f>MODE(A200:J200)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L200" s="16">
@@ -8345,7 +8345,7 @@
         <v>9</v>
       </c>
       <c r="K201" s="8">
-        <f>MODE(A201:J201)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L201" s="16">
@@ -8384,7 +8384,7 @@
         <v>2</v>
       </c>
       <c r="K202" s="8">
-        <f>MODE(A202:J202)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L202" s="16">
@@ -8423,7 +8423,7 @@
         <v>3</v>
       </c>
       <c r="K203" s="8">
-        <f>MODE(A203:J203)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L203" s="16">
@@ -8462,7 +8462,7 @@
         <v>6</v>
       </c>
       <c r="K204" s="8">
-        <f>MODE(A204:J204)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L204" s="16">
@@ -8501,7 +8501,7 @@
         <v>1</v>
       </c>
       <c r="K205" s="8">
-        <f>MODE(A205:J205)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L205" s="16">
@@ -8540,7 +8540,7 @@
         <v>1</v>
       </c>
       <c r="K206" s="8">
-        <f>MODE(A206:J206)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L206" s="16">
@@ -8579,7 +8579,7 @@
         <v>7</v>
       </c>
       <c r="K207" s="8">
-        <f>MODE(A207:J207)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L207" s="16">
@@ -8618,7 +8618,7 @@
         <v>8</v>
       </c>
       <c r="K208" s="8">
-        <f>MODE(A208:J208)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L208" s="16">
@@ -8657,7 +8657,7 @@
         <v>9</v>
       </c>
       <c r="K209" s="8">
-        <f>MODE(A209:J209)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L209" s="16">
@@ -8696,7 +8696,7 @@
         <v>5</v>
       </c>
       <c r="K210" s="8">
-        <f>MODE(A210:J210)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L210" s="16">
@@ -8735,7 +8735,7 @@
         <v>2</v>
       </c>
       <c r="K211" s="8">
-        <f>MODE(A211:J211)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L211" s="16">
@@ -8774,7 +8774,7 @@
         <v>5</v>
       </c>
       <c r="K212" s="8">
-        <f>MODE(A212:J212)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L212" s="16">
@@ -8813,7 +8813,7 @@
         <v>4</v>
       </c>
       <c r="K213" s="8">
-        <f>MODE(A213:J213)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L213" s="16">
@@ -8852,7 +8852,7 @@
         <v>8</v>
       </c>
       <c r="K214" s="8">
-        <f>MODE(A214:J214)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L214" s="16">
@@ -8891,7 +8891,7 @@
         <v>9</v>
       </c>
       <c r="K215" s="8">
-        <f>MODE(A215:J215)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L215" s="16">
@@ -8930,7 +8930,7 @@
         <v>3</v>
       </c>
       <c r="K216" s="8">
-        <f>MODE(A216:J216)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L216" s="16">
@@ -8947,7 +8947,9 @@
       <c r="C217" s="2">
         <v>9</v>
       </c>
-      <c r="D217" s="4"/>
+      <c r="D217" s="4">
+        <v>3</v>
+      </c>
       <c r="E217" s="4">
         <v>3</v>
       </c>
@@ -8967,7 +8969,7 @@
         <v>5</v>
       </c>
       <c r="K217" s="8">
-        <f>MODE(A217:J217)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L217" s="16">
@@ -9006,7 +9008,7 @@
         <v>0</v>
       </c>
       <c r="K218" s="8">
-        <f>MODE(A218:J218)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L218" s="16">
@@ -9045,7 +9047,7 @@
         <v>3</v>
       </c>
       <c r="K219" s="8">
-        <f>MODE(A219:J219)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L219" s="16">
@@ -9084,7 +9086,7 @@
         <v>6</v>
       </c>
       <c r="K220" s="8">
-        <f>MODE(A220:J220)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L220" s="16">
@@ -9123,7 +9125,7 @@
         <v>5</v>
       </c>
       <c r="K221" s="8">
-        <f>MODE(A221:J221)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L221" s="16">
@@ -9162,7 +9164,7 @@
         <v>5</v>
       </c>
       <c r="K222" s="8">
-        <f>MODE(A222:J222)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L222" s="16">
@@ -9201,7 +9203,7 @@
         <v>2</v>
       </c>
       <c r="K223" s="8">
-        <f>MODE(A223:J223)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L223" s="16">
@@ -9240,7 +9242,7 @@
         <v>6</v>
       </c>
       <c r="K224" s="8">
-        <f>MODE(A224:J224)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L224" s="16">
@@ -9279,7 +9281,7 @@
         <v>2</v>
       </c>
       <c r="K225" s="8">
-        <f>MODE(A225:J225)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L225" s="16">
@@ -9318,7 +9320,7 @@
         <v>7</v>
       </c>
       <c r="K226" s="8">
-        <f>MODE(A226:J226)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L226" s="16">
@@ -9357,7 +9359,7 @@
         <v>6</v>
       </c>
       <c r="K227" s="8">
-        <f>MODE(A227:J227)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L227" s="16">
@@ -9396,7 +9398,7 @@
         <v>2</v>
       </c>
       <c r="K228" s="8">
-        <f>MODE(A228:J228)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L228" s="16">
@@ -9435,7 +9437,7 @@
         <v>8</v>
       </c>
       <c r="K229" s="8">
-        <f>MODE(A229:J229)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L229" s="16">
@@ -9474,7 +9476,7 @@
         <v>4</v>
       </c>
       <c r="K230" s="8">
-        <f>MODE(A230:J230)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L230" s="16">
@@ -9513,7 +9515,7 @@
         <v>1</v>
       </c>
       <c r="K231" s="8">
-        <f>MODE(A231:J231)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L231" s="16">
@@ -9552,7 +9554,7 @@
         <v>7</v>
       </c>
       <c r="K232" s="8">
-        <f>MODE(A232:J232)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L232" s="16">
@@ -9591,7 +9593,7 @@
         <v>8</v>
       </c>
       <c r="K233" s="8">
-        <f>MODE(A233:J233)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L233" s="16">
@@ -9630,7 +9632,7 @@
         <v>8</v>
       </c>
       <c r="K234" s="8">
-        <f>MODE(A234:J234)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L234" s="16">
@@ -9669,7 +9671,7 @@
         <v>8</v>
       </c>
       <c r="K235" s="8">
-        <f>MODE(A235:J235)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L235" s="16">
@@ -9708,7 +9710,7 @@
         <v>8</v>
       </c>
       <c r="K236" s="8">
-        <f>MODE(A236:J236)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L236" s="16">
@@ -9747,7 +9749,7 @@
         <v>7</v>
       </c>
       <c r="K237" s="8">
-        <f>MODE(A237:J237)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L237" s="16">
@@ -9786,7 +9788,7 @@
         <v>9</v>
       </c>
       <c r="K238" s="8">
-        <f>MODE(A238:J238)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L238" s="16">
@@ -9825,7 +9827,7 @@
         <v>2</v>
       </c>
       <c r="K239" s="8">
-        <f>MODE(A239:J239)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L239" s="16">
@@ -9864,7 +9866,7 @@
         <v>2</v>
       </c>
       <c r="K240" s="8">
-        <f>MODE(A240:J240)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L240" s="16">
@@ -9903,7 +9905,7 @@
         <v>4</v>
       </c>
       <c r="K241" s="8">
-        <f>MODE(A241:J241)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L241" s="16">
@@ -9942,7 +9944,7 @@
         <v>1</v>
       </c>
       <c r="K242" s="8">
-        <f>MODE(A242:J242)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L242" s="16">
@@ -9981,7 +9983,7 @@
         <v>8</v>
       </c>
       <c r="K243" s="8">
-        <f>MODE(A243:J243)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L243" s="16">
@@ -10020,7 +10022,7 @@
         <v>5</v>
       </c>
       <c r="K244" s="8">
-        <f>MODE(A244:J244)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L244" s="16">
@@ -10059,7 +10061,7 @@
         <v>8</v>
       </c>
       <c r="K245" s="8">
-        <f>MODE(A245:J245)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L245" s="16">
@@ -10098,7 +10100,7 @@
         <v>7</v>
       </c>
       <c r="K246" s="8">
-        <f>MODE(A246:J246)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L246" s="16">
@@ -10137,7 +10139,7 @@
         <v>2</v>
       </c>
       <c r="K247" s="8">
-        <f>MODE(A247:J247)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L247" s="16">
@@ -10176,7 +10178,7 @@
         <v>3</v>
       </c>
       <c r="K248" s="8">
-        <f>MODE(A248:J248)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L248" s="16">
@@ -10215,7 +10217,7 @@
         <v>0</v>
       </c>
       <c r="K249" s="8">
-        <f>MODE(A249:J249)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L249" s="16">
@@ -10254,7 +10256,7 @@
         <v>4</v>
       </c>
       <c r="K250" s="8">
-        <f>MODE(A250:J250)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L250" s="16">
@@ -10293,7 +10295,7 @@
         <v>4</v>
       </c>
       <c r="K251" s="8">
-        <f>MODE(A251:J251)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L251" s="16">
@@ -10332,7 +10334,7 @@
         <v>2</v>
       </c>
       <c r="K252" s="8">
-        <f>MODE(A252:J252)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L252" s="16">
@@ -10371,7 +10373,7 @@
         <v>4</v>
       </c>
       <c r="K253" s="8">
-        <f>MODE(A253:J253)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L253" s="16">
@@ -10410,7 +10412,7 @@
         <v>1</v>
       </c>
       <c r="K254" s="8">
-        <f>MODE(A254:J254)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L254" s="16">
@@ -10449,7 +10451,7 @@
         <v>9</v>
       </c>
       <c r="K255" s="8">
-        <f>MODE(A255:J255)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L255" s="16">
@@ -10488,7 +10490,7 @@
         <v>5</v>
       </c>
       <c r="K256" s="8">
-        <f>MODE(A256:J256)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L256" s="16">
@@ -10527,7 +10529,7 @@
         <v>7</v>
       </c>
       <c r="K257" s="8">
-        <f>MODE(A257:J257)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L257" s="16">
@@ -10566,7 +10568,7 @@
         <v>7</v>
       </c>
       <c r="K258" s="8">
-        <f>MODE(A258:J258)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L258" s="16">
@@ -10605,7 +10607,7 @@
         <v>2</v>
       </c>
       <c r="K259" s="8">
-        <f>MODE(A259:J259)</f>
+        <f t="shared" ref="K259:K322" si="4">MODE(A259:J259)</f>
         <v>2</v>
       </c>
       <c r="L259" s="16">
@@ -10644,7 +10646,7 @@
         <v>8</v>
       </c>
       <c r="K260" s="8">
-        <f>MODE(A260:J260)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L260" s="16">
@@ -10683,7 +10685,7 @@
         <v>2</v>
       </c>
       <c r="K261" s="8">
-        <f>MODE(A261:J261)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L261" s="16">
@@ -10722,7 +10724,7 @@
         <v>6</v>
       </c>
       <c r="K262" s="8">
-        <f>MODE(A262:J262)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L262" s="16">
@@ -10761,7 +10763,7 @@
         <v>8</v>
       </c>
       <c r="K263" s="8">
-        <f>MODE(A263:J263)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L263" s="16">
@@ -10800,7 +10802,7 @@
         <v>5</v>
       </c>
       <c r="K264" s="8">
-        <f>MODE(A264:J264)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L264" s="16">
@@ -10839,7 +10841,7 @@
         <v>7</v>
       </c>
       <c r="K265" s="8">
-        <f>MODE(A265:J265)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L265" s="16">
@@ -10878,7 +10880,7 @@
         <v>7</v>
       </c>
       <c r="K266" s="8">
-        <f>MODE(A266:J266)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L266" s="16">
@@ -10917,7 +10919,7 @@
         <v>9</v>
       </c>
       <c r="K267" s="8">
-        <f>MODE(A267:J267)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L267" s="16">
@@ -10956,7 +10958,7 @@
         <v>1</v>
       </c>
       <c r="K268" s="8">
-        <f>MODE(A268:J268)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L268" s="16">
@@ -10995,7 +10997,7 @@
         <v>8</v>
       </c>
       <c r="K269" s="8">
-        <f>MODE(A269:J269)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L269" s="16">
@@ -11034,7 +11036,7 @@
         <v>1</v>
       </c>
       <c r="K270" s="8">
-        <f>MODE(A270:J270)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L270" s="16">
@@ -11073,7 +11075,7 @@
         <v>8</v>
       </c>
       <c r="K271" s="8">
-        <f>MODE(A271:J271)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L271" s="16">
@@ -11112,7 +11114,7 @@
         <v>0</v>
       </c>
       <c r="K272" s="8">
-        <f>MODE(A272:J272)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L272" s="16">
@@ -11151,7 +11153,7 @@
         <v>3</v>
       </c>
       <c r="K273" s="8">
-        <f>MODE(A273:J273)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L273" s="16">
@@ -11190,7 +11192,7 @@
         <v>0</v>
       </c>
       <c r="K274" s="8">
-        <f>MODE(A274:J274)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L274" s="16">
@@ -11229,7 +11231,7 @@
         <v>1</v>
       </c>
       <c r="K275" s="8">
-        <f>MODE(A275:J275)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L275" s="16">
@@ -11268,7 +11270,7 @@
         <v>9</v>
       </c>
       <c r="K276" s="8">
-        <f>MODE(A276:J276)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L276" s="16">
@@ -11307,7 +11309,7 @@
         <v>9</v>
       </c>
       <c r="K277" s="8">
-        <f>MODE(A277:J277)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L277" s="16">
@@ -11346,7 +11348,7 @@
         <v>4</v>
       </c>
       <c r="K278" s="8">
-        <f>MODE(A278:J278)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L278" s="16">
@@ -11385,7 +11387,7 @@
         <v>1</v>
       </c>
       <c r="K279" s="8">
-        <f>MODE(A279:J279)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L279" s="16">
@@ -11424,7 +11426,7 @@
         <v>8</v>
       </c>
       <c r="K280" s="8">
-        <f>MODE(A280:J280)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L280" s="16">
@@ -11463,7 +11465,7 @@
         <v>2</v>
       </c>
       <c r="K281" s="8">
-        <f>MODE(A281:J281)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L281" s="16">
@@ -11502,7 +11504,7 @@
         <v>1</v>
       </c>
       <c r="K282" s="8">
-        <f>MODE(A282:J282)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L282" s="16">
@@ -11541,7 +11543,7 @@
         <v>2</v>
       </c>
       <c r="K283" s="8">
-        <f>MODE(A283:J283)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L283" s="16">
@@ -11580,7 +11582,7 @@
         <v>9</v>
       </c>
       <c r="K284" s="8">
-        <f>MODE(A284:J284)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L284" s="16">
@@ -11619,7 +11621,7 @@
         <v>7</v>
       </c>
       <c r="K285" s="8">
-        <f>MODE(A285:J285)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L285" s="16">
@@ -11658,7 +11660,7 @@
         <v>5</v>
       </c>
       <c r="K286" s="8">
-        <f>MODE(A286:J286)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L286" s="16">
@@ -11697,7 +11699,7 @@
         <v>9</v>
       </c>
       <c r="K287" s="8">
-        <f>MODE(A287:J287)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L287" s="16">
@@ -11736,7 +11738,7 @@
         <v>2</v>
       </c>
       <c r="K288" s="8">
-        <f>MODE(A288:J288)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L288" s="16">
@@ -11775,7 +11777,7 @@
         <v>6</v>
       </c>
       <c r="K289" s="8">
-        <f>MODE(A289:J289)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L289" s="16">
@@ -11814,7 +11816,7 @@
         <v>4</v>
       </c>
       <c r="K290" s="8">
-        <f>MODE(A290:J290)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L290" s="16">
@@ -11853,7 +11855,7 @@
         <v>1</v>
       </c>
       <c r="K291" s="8">
-        <f>MODE(A291:J291)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L291" s="16">
@@ -11892,7 +11894,7 @@
         <v>5</v>
       </c>
       <c r="K292" s="8">
-        <f>MODE(A292:J292)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L292" s="16">
@@ -11931,7 +11933,7 @@
         <v>8</v>
       </c>
       <c r="K293" s="8">
-        <f>MODE(A293:J293)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L293" s="16">
@@ -11970,7 +11972,7 @@
         <v>2</v>
       </c>
       <c r="K294" s="8">
-        <f>MODE(A294:J294)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L294" s="16">
@@ -12009,7 +12011,7 @@
         <v>9</v>
       </c>
       <c r="K295" s="8">
-        <f>MODE(A295:J295)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L295" s="16">
@@ -12048,7 +12050,7 @@
         <v>2</v>
       </c>
       <c r="K296" s="8">
-        <f>MODE(A296:J296)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L296" s="16">
@@ -12087,7 +12089,7 @@
         <v>0</v>
       </c>
       <c r="K297" s="8">
-        <f>MODE(A297:J297)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L297" s="16">
@@ -12126,7 +12128,7 @@
         <v>4</v>
       </c>
       <c r="K298" s="8">
-        <f>MODE(A298:J298)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L298" s="16">
@@ -12165,7 +12167,7 @@
         <v>0</v>
       </c>
       <c r="K299" s="8">
-        <f>MODE(A299:J299)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L299" s="16">
@@ -12204,7 +12206,7 @@
         <v>0</v>
       </c>
       <c r="K300" s="8">
-        <f>MODE(A300:J300)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L300" s="16">
@@ -12243,7 +12245,7 @@
         <v>2</v>
       </c>
       <c r="K301" s="8">
-        <f>MODE(A301:J301)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L301" s="16">
@@ -12282,7 +12284,7 @@
         <v>8</v>
       </c>
       <c r="K302" s="8">
-        <f>MODE(A302:J302)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L302" s="16">
@@ -12321,7 +12323,7 @@
         <v>4</v>
       </c>
       <c r="K303" s="8">
-        <f>MODE(A303:J303)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L303" s="16">
@@ -12360,7 +12362,7 @@
         <v>7</v>
       </c>
       <c r="K304" s="8">
-        <f>MODE(A304:J304)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L304" s="16">
@@ -12399,7 +12401,7 @@
         <v>1</v>
       </c>
       <c r="K305" s="8">
-        <f>MODE(A305:J305)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L305" s="16">
@@ -12438,7 +12440,7 @@
         <v>2</v>
       </c>
       <c r="K306" s="8">
-        <f>MODE(A306:J306)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L306" s="16">
@@ -12477,7 +12479,7 @@
         <v>4</v>
       </c>
       <c r="K307" s="8">
-        <f>MODE(A307:J307)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L307" s="16">
@@ -12516,7 +12518,7 @@
         <v>0</v>
       </c>
       <c r="K308" s="8">
-        <f>MODE(A308:J308)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L308" s="16">
@@ -12555,7 +12557,7 @@
         <v>2</v>
       </c>
       <c r="K309" s="8">
-        <f>MODE(A309:J309)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L309" s="16">
@@ -12594,7 +12596,7 @@
         <v>7</v>
       </c>
       <c r="K310" s="8">
-        <f>MODE(A310:J310)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="L310" s="16">
@@ -12633,7 +12635,7 @@
         <v>8</v>
       </c>
       <c r="K311" s="8">
-        <f>MODE(A311:J311)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="L311" s="16">
@@ -12672,7 +12674,7 @@
         <v>3</v>
       </c>
       <c r="K312" s="8">
-        <f>MODE(A312:J312)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L312" s="16">
@@ -12711,7 +12713,7 @@
         <v>3</v>
       </c>
       <c r="K313" s="8">
-        <f>MODE(A313:J313)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L313" s="16">
@@ -12750,7 +12752,7 @@
         <v>0</v>
       </c>
       <c r="K314" s="8">
-        <f>MODE(A314:J314)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L314" s="16">
@@ -12789,7 +12791,7 @@
         <v>0</v>
       </c>
       <c r="K315" s="8">
-        <f>MODE(A315:J315)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L315" s="16">
@@ -12828,7 +12830,7 @@
         <v>3</v>
       </c>
       <c r="K316" s="8">
-        <f>MODE(A316:J316)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L316" s="16">
@@ -12867,7 +12869,7 @@
         <v>1</v>
       </c>
       <c r="K317" s="8">
-        <f>MODE(A317:J317)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L317" s="16">
@@ -12906,7 +12908,7 @@
         <v>9</v>
       </c>
       <c r="K318" s="8">
-        <f>MODE(A318:J318)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="L318" s="16">
@@ -12945,7 +12947,7 @@
         <v>6</v>
       </c>
       <c r="K319" s="8">
-        <f>MODE(A319:J319)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L319" s="16">
@@ -12984,7 +12986,7 @@
         <v>5</v>
       </c>
       <c r="K320" s="8">
-        <f>MODE(A320:J320)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L320" s="16">
@@ -13023,7 +13025,7 @@
         <v>8</v>
       </c>
       <c r="K321" s="8">
-        <f>MODE(A321:J321)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L321" s="16">
@@ -13062,7 +13064,7 @@
         <v>5</v>
       </c>
       <c r="K322" s="8">
-        <f>MODE(A322:J322)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L322" s="16">
@@ -13101,7 +13103,7 @@
         <v>1</v>
       </c>
       <c r="K323" s="8">
-        <f>MODE(A323:J323)</f>
+        <f t="shared" ref="K323:K386" si="5">MODE(A323:J323)</f>
         <v>9</v>
       </c>
       <c r="L323" s="16">
@@ -13140,7 +13142,7 @@
         <v>2</v>
       </c>
       <c r="K324" s="8">
-        <f>MODE(A324:J324)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L324" s="16">
@@ -13179,7 +13181,7 @@
         <v>9</v>
       </c>
       <c r="K325" s="8">
-        <f>MODE(A325:J325)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="L325" s="16">
@@ -13218,7 +13220,7 @@
         <v>3</v>
       </c>
       <c r="K326" s="8">
-        <f>MODE(A326:J326)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L326" s="16">
@@ -13257,7 +13259,7 @@
         <v>0</v>
       </c>
       <c r="K327" s="8">
-        <f>MODE(A327:J327)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L327" s="16">
@@ -13296,7 +13298,7 @@
         <v>4</v>
       </c>
       <c r="K328" s="8">
-        <f>MODE(A328:J328)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L328" s="16">
@@ -13335,7 +13337,7 @@
         <v>2</v>
       </c>
       <c r="K329" s="8">
-        <f>MODE(A329:J329)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L329" s="16">
@@ -13374,7 +13376,7 @@
         <v>0</v>
       </c>
       <c r="K330" s="8">
-        <f>MODE(A330:J330)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L330" s="16">
@@ -13413,7 +13415,7 @@
         <v>7</v>
       </c>
       <c r="K331" s="8">
-        <f>MODE(A331:J331)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L331" s="16">
@@ -13452,7 +13454,7 @@
         <v>1</v>
       </c>
       <c r="K332" s="8">
-        <f>MODE(A332:J332)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L332" s="16">
@@ -13491,7 +13493,7 @@
         <v>1</v>
       </c>
       <c r="K333" s="8">
-        <f>MODE(A333:J333)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L333" s="16">
@@ -13530,7 +13532,7 @@
         <v>2</v>
       </c>
       <c r="K334" s="8">
-        <f>MODE(A334:J334)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L334" s="16">
@@ -13569,7 +13571,7 @@
         <v>1</v>
       </c>
       <c r="K335" s="8">
-        <f>MODE(A335:J335)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L335" s="16">
@@ -13608,7 +13610,7 @@
         <v>5</v>
       </c>
       <c r="K336" s="8">
-        <f>MODE(A336:J336)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L336" s="16">
@@ -13647,7 +13649,7 @@
         <v>3</v>
       </c>
       <c r="K337" s="8">
-        <f>MODE(A337:J337)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L337" s="16">
@@ -13686,7 +13688,7 @@
         <v>3</v>
       </c>
       <c r="K338" s="8">
-        <f>MODE(A338:J338)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L338" s="16">
@@ -13725,7 +13727,7 @@
         <v>4</v>
       </c>
       <c r="K339" s="8">
-        <f>MODE(A339:J339)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="L339" s="16">
@@ -13764,7 +13766,7 @@
         <v>2</v>
       </c>
       <c r="K340" s="8">
-        <f>MODE(A340:J340)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L340" s="16">
@@ -13803,7 +13805,7 @@
         <v>8</v>
       </c>
       <c r="K341" s="8">
-        <f>MODE(A341:J341)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L341" s="16">
@@ -13842,7 +13844,7 @@
         <v>6</v>
       </c>
       <c r="K342" s="8">
-        <f>MODE(A342:J342)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L342" s="16">
@@ -13881,7 +13883,7 @@
         <v>8</v>
       </c>
       <c r="K343" s="8">
-        <f>MODE(A343:J343)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L343" s="16">
@@ -13920,7 +13922,7 @@
         <v>6</v>
       </c>
       <c r="K344" s="8">
-        <f>MODE(A344:J344)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L344" s="16">
@@ -13959,7 +13961,7 @@
         <v>1</v>
       </c>
       <c r="K345" s="8">
-        <f>MODE(A345:J345)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L345" s="16">
@@ -13998,7 +14000,7 @@
         <v>3</v>
       </c>
       <c r="K346" s="8">
-        <f>MODE(A346:J346)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L346" s="16">
@@ -14037,7 +14039,7 @@
         <v>8</v>
       </c>
       <c r="K347" s="8">
-        <f>MODE(A347:J347)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L347" s="16">
@@ -14076,7 +14078,7 @@
         <v>1</v>
       </c>
       <c r="K348" s="8">
-        <f>MODE(A348:J348)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L348" s="16">
@@ -14115,7 +14117,7 @@
         <v>0</v>
       </c>
       <c r="K349" s="8">
-        <f>MODE(A349:J349)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L349" s="16">
@@ -14154,7 +14156,7 @@
         <v>5</v>
       </c>
       <c r="K350" s="8">
-        <f>MODE(A350:J350)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L350" s="16">
@@ -14193,7 +14195,7 @@
         <v>1</v>
       </c>
       <c r="K351" s="8">
-        <f>MODE(A351:J351)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L351" s="16">
@@ -14232,7 +14234,7 @@
         <v>3</v>
       </c>
       <c r="K352" s="8">
-        <f>MODE(A352:J352)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L352" s="16">
@@ -14271,7 +14273,7 @@
         <v>1</v>
       </c>
       <c r="K353" s="8">
-        <f>MODE(A353:J353)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L353" s="16">
@@ -14310,7 +14312,7 @@
         <v>5</v>
       </c>
       <c r="K354" s="8">
-        <f>MODE(A354:J354)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L354" s="16">
@@ -14349,7 +14351,7 @@
         <v>5</v>
       </c>
       <c r="K355" s="8">
-        <f>MODE(A355:J355)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L355" s="16">
@@ -14388,7 +14390,7 @@
         <v>6</v>
       </c>
       <c r="K356" s="8">
-        <f>MODE(A356:J356)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L356" s="16">
@@ -14427,7 +14429,7 @@
         <v>1</v>
       </c>
       <c r="K357" s="8">
-        <f>MODE(A357:J357)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L357" s="16">
@@ -14466,7 +14468,7 @@
         <v>8</v>
       </c>
       <c r="K358" s="8">
-        <f>MODE(A358:J358)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L358" s="16">
@@ -14505,7 +14507,7 @@
         <v>5</v>
       </c>
       <c r="K359" s="8">
-        <f>MODE(A359:J359)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L359" s="16">
@@ -14544,7 +14546,7 @@
         <v>1</v>
       </c>
       <c r="K360" s="8">
-        <f>MODE(A360:J360)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L360" s="16">
@@ -14583,7 +14585,7 @@
         <v>4</v>
       </c>
       <c r="K361" s="8">
-        <f>MODE(A361:J361)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L361" s="16">
@@ -14600,7 +14602,9 @@
       <c r="C362" s="2">
         <v>9</v>
       </c>
-      <c r="D362" s="4"/>
+      <c r="D362" s="4">
+        <v>9</v>
+      </c>
       <c r="E362" s="4">
         <v>4</v>
       </c>
@@ -14620,7 +14624,7 @@
         <v>4</v>
       </c>
       <c r="K362" s="8">
-        <f>MODE(A362:J362)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L362" s="16">
@@ -14659,7 +14663,7 @@
         <v>4</v>
       </c>
       <c r="K363" s="8">
-        <f>MODE(A363:J363)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L363" s="16">
@@ -14698,7 +14702,7 @@
         <v>6</v>
       </c>
       <c r="K364" s="8">
-        <f>MODE(A364:J364)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L364" s="16">
@@ -14737,7 +14741,7 @@
         <v>2</v>
       </c>
       <c r="K365" s="8">
-        <f>MODE(A365:J365)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L365" s="16">
@@ -14776,7 +14780,7 @@
         <v>2</v>
       </c>
       <c r="K366" s="8">
-        <f>MODE(A366:J366)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L366" s="16">
@@ -14815,7 +14819,7 @@
         <v>5</v>
       </c>
       <c r="K367" s="8">
-        <f>MODE(A367:J367)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L367" s="16">
@@ -14854,7 +14858,7 @@
         <v>0</v>
       </c>
       <c r="K368" s="8">
-        <f>MODE(A368:J368)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L368" s="16">
@@ -14893,7 +14897,7 @@
         <v>6</v>
       </c>
       <c r="K369" s="8">
-        <f>MODE(A369:J369)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L369" s="16">
@@ -14932,7 +14936,7 @@
         <v>5</v>
       </c>
       <c r="K370" s="8">
-        <f>MODE(A370:J370)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L370" s="16">
@@ -14971,7 +14975,7 @@
         <v>6</v>
       </c>
       <c r="K371" s="8">
-        <f>MODE(A371:J371)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L371" s="16">
@@ -15010,7 +15014,7 @@
         <v>3</v>
       </c>
       <c r="K372" s="8">
-        <f>MODE(A372:J372)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L372" s="16">
@@ -15049,7 +15053,7 @@
         <v>7</v>
       </c>
       <c r="K373" s="8">
-        <f>MODE(A373:J373)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L373" s="16">
@@ -15088,7 +15092,7 @@
         <v>2</v>
       </c>
       <c r="K374" s="8">
-        <f>MODE(A374:J374)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L374" s="16">
@@ -15127,7 +15131,7 @@
         <v>0</v>
       </c>
       <c r="K375" s="8">
-        <f>MODE(A375:J375)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L375" s="16">
@@ -15166,7 +15170,7 @@
         <v>8</v>
       </c>
       <c r="K376" s="8">
-        <f>MODE(A376:J376)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L376" s="16">
@@ -15205,7 +15209,7 @@
         <v>8</v>
       </c>
       <c r="K377" s="8">
-        <f>MODE(A377:J377)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L377" s="16">
@@ -15244,7 +15248,7 @@
         <v>5</v>
       </c>
       <c r="K378" s="8">
-        <f>MODE(A378:J378)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L378" s="16">
@@ -15283,7 +15287,7 @@
         <v>4</v>
       </c>
       <c r="K379" s="8">
-        <f>MODE(A379:J379)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L379" s="16">
@@ -15322,7 +15326,7 @@
         <v>1</v>
       </c>
       <c r="K380" s="8">
-        <f>MODE(A380:J380)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L380" s="16">
@@ -15361,7 +15365,7 @@
         <v>1</v>
       </c>
       <c r="K381" s="8">
-        <f>MODE(A381:J381)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L381" s="16">
@@ -15400,7 +15404,7 @@
         <v>4</v>
       </c>
       <c r="K382" s="8">
-        <f>MODE(A382:J382)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L382" s="16">
@@ -15439,7 +15443,7 @@
         <v>0</v>
       </c>
       <c r="K383" s="8">
-        <f>MODE(A383:J383)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L383" s="16">
@@ -15478,7 +15482,7 @@
         <v>3</v>
       </c>
       <c r="K384" s="8">
-        <f>MODE(A384:J384)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L384" s="16">
@@ -15517,7 +15521,7 @@
         <v>3</v>
       </c>
       <c r="K385" s="8">
-        <f>MODE(A385:J385)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L385" s="16">
@@ -15556,7 +15560,7 @@
         <v>7</v>
       </c>
       <c r="K386" s="8">
-        <f>MODE(A386:J386)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L386" s="16">
@@ -15595,7 +15599,7 @@
         <v>6</v>
       </c>
       <c r="K387" s="8">
-        <f>MODE(A387:J387)</f>
+        <f t="shared" ref="K387:K450" si="6">MODE(A387:J387)</f>
         <v>6</v>
       </c>
       <c r="L387" s="16">
@@ -15634,7 +15638,7 @@
         <v>1</v>
       </c>
       <c r="K388" s="8">
-        <f>MODE(A388:J388)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L388" s="16">
@@ -15673,7 +15677,7 @@
         <v>6</v>
       </c>
       <c r="K389" s="8">
-        <f>MODE(A389:J389)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L389" s="16">
@@ -15712,7 +15716,7 @@
         <v>2</v>
       </c>
       <c r="K390" s="8">
-        <f>MODE(A390:J390)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L390" s="16">
@@ -15751,7 +15755,7 @@
         <v>1</v>
       </c>
       <c r="K391" s="8">
-        <f>MODE(A391:J391)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L391" s="16">
@@ -15790,7 +15794,7 @@
         <v>9</v>
       </c>
       <c r="K392" s="8">
-        <f>MODE(A392:J392)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L392" s="16">
@@ -15829,7 +15833,7 @@
         <v>2</v>
       </c>
       <c r="K393" s="8">
-        <f>MODE(A393:J393)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L393" s="16">
@@ -15868,7 +15872,7 @@
         <v>8</v>
       </c>
       <c r="K394" s="8">
-        <f>MODE(A394:J394)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L394" s="16">
@@ -15907,7 +15911,7 @@
         <v>6</v>
       </c>
       <c r="K395" s="8">
-        <f>MODE(A395:J395)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L395" s="16">
@@ -15946,7 +15950,7 @@
         <v>1</v>
       </c>
       <c r="K396" s="8">
-        <f>MODE(A396:J396)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L396" s="16">
@@ -15985,7 +15989,7 @@
         <v>4</v>
       </c>
       <c r="K397" s="8">
-        <f>MODE(A397:J397)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L397" s="16">
@@ -16024,7 +16028,7 @@
         <v>5</v>
       </c>
       <c r="K398" s="8">
-        <f>MODE(A398:J398)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="L398" s="16">
@@ -16063,7 +16067,7 @@
         <v>2</v>
       </c>
       <c r="K399" s="8">
-        <f>MODE(A399:J399)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L399" s="16">
@@ -16102,7 +16106,7 @@
         <v>8</v>
       </c>
       <c r="K400" s="8">
-        <f>MODE(A400:J400)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L400" s="16">
@@ -16141,7 +16145,7 @@
         <v>4</v>
       </c>
       <c r="K401" s="8">
-        <f>MODE(A401:J401)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L401" s="16">
@@ -16180,7 +16184,7 @@
         <v>9</v>
       </c>
       <c r="K402" s="8">
-        <f>MODE(A402:J402)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L402" s="16">
@@ -16219,7 +16223,7 @@
         <v>2</v>
       </c>
       <c r="K403" s="8">
-        <f>MODE(A403:J403)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L403" s="16">
@@ -16258,7 +16262,7 @@
         <v>8</v>
       </c>
       <c r="K404" s="8">
-        <f>MODE(A404:J404)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L404" s="16">
@@ -16297,7 +16301,7 @@
         <v>3</v>
       </c>
       <c r="K405" s="8">
-        <f>MODE(A405:J405)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L405" s="16">
@@ -16336,7 +16340,7 @@
         <v>8</v>
       </c>
       <c r="K406" s="8">
-        <f>MODE(A406:J406)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L406" s="16">
@@ -16375,7 +16379,7 @@
         <v>2</v>
       </c>
       <c r="K407" s="8">
-        <f>MODE(A407:J407)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L407" s="16">
@@ -16414,7 +16418,7 @@
         <v>4</v>
       </c>
       <c r="K408" s="8">
-        <f>MODE(A408:J408)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L408" s="16">
@@ -16453,7 +16457,7 @@
         <v>5</v>
       </c>
       <c r="K409" s="8">
-        <f>MODE(A409:J409)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="L409" s="16">
@@ -16492,7 +16496,7 @@
         <v>0</v>
       </c>
       <c r="K410" s="8">
-        <f>MODE(A410:J410)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L410" s="16">
@@ -16531,7 +16535,7 @@
         <v>3</v>
       </c>
       <c r="K411" s="8">
-        <f>MODE(A411:J411)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L411" s="16">
@@ -16570,7 +16574,7 @@
         <v>1</v>
       </c>
       <c r="K412" s="8">
-        <f>MODE(A412:J412)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L412" s="16">
@@ -16609,7 +16613,7 @@
         <v>7</v>
       </c>
       <c r="K413" s="8">
-        <f>MODE(A413:J413)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L413" s="16">
@@ -16648,7 +16652,7 @@
         <v>7</v>
       </c>
       <c r="K414" s="8">
-        <f>MODE(A414:J414)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L414" s="16">
@@ -16687,7 +16691,7 @@
         <v>5</v>
       </c>
       <c r="K415" s="8">
-        <f>MODE(A415:J415)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="L415" s="16">
@@ -16726,7 +16730,7 @@
         <v>7</v>
       </c>
       <c r="K416" s="8">
-        <f>MODE(A416:J416)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L416" s="16">
@@ -16765,7 +16769,7 @@
         <v>9</v>
       </c>
       <c r="K417" s="8">
-        <f>MODE(A417:J417)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L417" s="16">
@@ -16804,7 +16808,7 @@
         <v>7</v>
       </c>
       <c r="K418" s="8">
-        <f>MODE(A418:J418)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L418" s="16">
@@ -16843,7 +16847,7 @@
         <v>7</v>
       </c>
       <c r="K419" s="8">
-        <f>MODE(A419:J419)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L419" s="16">
@@ -16882,7 +16886,7 @@
         <v>4</v>
       </c>
       <c r="K420" s="8">
-        <f>MODE(A420:J420)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L420" s="16">
@@ -16921,7 +16925,7 @@
         <v>2</v>
       </c>
       <c r="K421" s="8">
-        <f>MODE(A421:J421)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L421" s="16">
@@ -16960,7 +16964,7 @@
         <v>1</v>
       </c>
       <c r="K422" s="8">
-        <f>MODE(A422:J422)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L422" s="16">
@@ -16999,7 +17003,7 @@
         <v>4</v>
       </c>
       <c r="K423" s="8">
-        <f>MODE(A423:J423)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L423" s="16">
@@ -17038,7 +17042,7 @@
         <v>2</v>
       </c>
       <c r="K424" s="8">
-        <f>MODE(A424:J424)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L424" s="16">
@@ -17077,7 +17081,7 @@
         <v>9</v>
       </c>
       <c r="K425" s="8">
-        <f>MODE(A425:J425)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L425" s="16">
@@ -17116,7 +17120,7 @@
         <v>2</v>
       </c>
       <c r="K426" s="8">
-        <f>MODE(A426:J426)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L426" s="16">
@@ -17155,7 +17159,7 @@
         <v>0</v>
       </c>
       <c r="K427" s="8">
-        <f>MODE(A427:J427)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L427" s="16">
@@ -17194,7 +17198,7 @@
         <v>4</v>
       </c>
       <c r="K428" s="8">
-        <f>MODE(A428:J428)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L428" s="16">
@@ -17233,7 +17237,7 @@
         <v>9</v>
       </c>
       <c r="K429" s="8">
-        <f>MODE(A429:J429)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L429" s="16">
@@ -17272,7 +17276,7 @@
         <v>1</v>
       </c>
       <c r="K430" s="8">
-        <f>MODE(A430:J430)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L430" s="16">
@@ -17311,7 +17315,7 @@
         <v>4</v>
       </c>
       <c r="K431" s="8">
-        <f>MODE(A431:J431)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L431" s="16">
@@ -17350,7 +17354,7 @@
         <v>8</v>
       </c>
       <c r="K432" s="8">
-        <f>MODE(A432:J432)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L432" s="16">
@@ -17389,7 +17393,7 @@
         <v>1</v>
       </c>
       <c r="K433" s="8">
-        <f>MODE(A433:J433)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L433" s="16">
@@ -17428,7 +17432,7 @@
         <v>8</v>
       </c>
       <c r="K434" s="8">
-        <f>MODE(A434:J434)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L434" s="16">
@@ -17467,7 +17471,7 @@
         <v>4</v>
       </c>
       <c r="K435" s="8">
-        <f>MODE(A435:J435)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L435" s="16">
@@ -17506,7 +17510,7 @@
         <v>5</v>
       </c>
       <c r="K436" s="8">
-        <f>MODE(A436:J436)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="L436" s="16">
@@ -17545,7 +17549,7 @@
         <v>9</v>
       </c>
       <c r="K437" s="8">
-        <f>MODE(A437:J437)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="L437" s="16">
@@ -17584,7 +17588,7 @@
         <v>8</v>
       </c>
       <c r="K438" s="8">
-        <f>MODE(A438:J438)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L438" s="16">
@@ -17623,7 +17627,7 @@
         <v>8</v>
       </c>
       <c r="K439" s="8">
-        <f>MODE(A439:J439)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="L439" s="16">
@@ -17662,7 +17666,7 @@
         <v>3</v>
       </c>
       <c r="K440" s="8">
-        <f>MODE(A440:J440)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L440" s="16">
@@ -17701,7 +17705,7 @@
         <v>7</v>
       </c>
       <c r="K441" s="8">
-        <f>MODE(A441:J441)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="L441" s="16">
@@ -17740,7 +17744,7 @@
         <v>6</v>
       </c>
       <c r="K442" s="8">
-        <f>MODE(A442:J442)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L442" s="16">
@@ -17779,7 +17783,7 @@
         <v>0</v>
       </c>
       <c r="K443" s="8">
-        <f>MODE(A443:J443)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L443" s="16">
@@ -17818,7 +17822,7 @@
         <v>0</v>
       </c>
       <c r="K444" s="8">
-        <f>MODE(A444:J444)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L444" s="16">
@@ -17857,7 +17861,7 @@
         <v>3</v>
       </c>
       <c r="K445" s="8">
-        <f>MODE(A445:J445)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L445" s="16">
@@ -17896,7 +17900,7 @@
         <v>0</v>
       </c>
       <c r="K446" s="8">
-        <f>MODE(A446:J446)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L446" s="16">
@@ -17935,7 +17939,7 @@
         <v>2</v>
       </c>
       <c r="K447" s="8">
-        <f>MODE(A447:J447)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L447" s="16">
@@ -17974,7 +17978,7 @@
         <v>6</v>
       </c>
       <c r="K448" s="8">
-        <f>MODE(A448:J448)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L448" s="16">
@@ -18013,7 +18017,7 @@
         <v>6</v>
       </c>
       <c r="K449" s="8">
-        <f>MODE(A449:J449)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L449" s="16">
@@ -18052,7 +18056,7 @@
         <v>4</v>
       </c>
       <c r="K450" s="8">
-        <f>MODE(A450:J450)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="L450" s="16">
@@ -18091,7 +18095,7 @@
         <v>5</v>
       </c>
       <c r="K451" s="8">
-        <f>MODE(A451:J451)</f>
+        <f t="shared" ref="K451:K514" si="7">MODE(A451:J451)</f>
         <v>9</v>
       </c>
       <c r="L451" s="16">
@@ -18130,7 +18134,7 @@
         <v>5</v>
       </c>
       <c r="K452" s="8">
-        <f>MODE(A452:J452)</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L452" s="16">
@@ -18169,7 +18173,7 @@
         <v>3</v>
       </c>
       <c r="K453" s="8">
-        <f>MODE(A453:J453)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L453" s="16">
@@ -18208,7 +18212,7 @@
         <v>3</v>
       </c>
       <c r="K454" s="8">
-        <f>MODE(A454:J454)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L454" s="16">
@@ -18247,7 +18251,7 @@
         <v>2</v>
       </c>
       <c r="K455" s="8">
-        <f>MODE(A455:J455)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="L455" s="16">
@@ -18286,7 +18290,7 @@
         <v>3</v>
       </c>
       <c r="K456" s="8">
-        <f>MODE(A456:J456)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L456" s="16">
@@ -18325,7 +18329,7 @@
         <v>9</v>
       </c>
       <c r="K457" s="8">
-        <f>MODE(A457:J457)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L457" s="16">
@@ -18364,7 +18368,7 @@
         <v>1</v>
       </c>
       <c r="K458" s="8">
-        <f>MODE(A458:J458)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L458" s="16">
@@ -18403,7 +18407,7 @@
         <v>2</v>
       </c>
       <c r="K459" s="8">
-        <f>MODE(A459:J459)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="L459" s="16">
@@ -18442,7 +18446,7 @@
         <v>6</v>
       </c>
       <c r="K460" s="8">
-        <f>MODE(A460:J460)</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L460" s="16">
@@ -18481,7 +18485,7 @@
         <v>8</v>
       </c>
       <c r="K461" s="8">
-        <f>MODE(A461:J461)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L461" s="16">
@@ -18520,7 +18524,7 @@
         <v>0</v>
       </c>
       <c r="K462" s="8">
-        <f>MODE(A462:J462)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L462" s="16">
@@ -18559,7 +18563,7 @@
         <v>5</v>
       </c>
       <c r="K463" s="8">
-        <f>MODE(A463:J463)</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L463" s="16">
@@ -18598,7 +18602,7 @@
         <v>6</v>
       </c>
       <c r="K464" s="8">
-        <f>MODE(A464:J464)</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L464" s="16">
@@ -18637,7 +18641,7 @@
         <v>6</v>
       </c>
       <c r="K465" s="8">
-        <f>MODE(A465:J465)</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L465" s="16">
@@ -18676,7 +18680,7 @@
         <v>6</v>
       </c>
       <c r="K466" s="8">
-        <f>MODE(A466:J466)</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L466" s="16">
@@ -18715,7 +18719,7 @@
         <v>6</v>
       </c>
       <c r="K467" s="8">
-        <f>MODE(A467:J467)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L467" s="16">
@@ -18754,7 +18758,7 @@
         <v>3</v>
       </c>
       <c r="K468" s="8">
-        <f>MODE(A468:J468)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L468" s="16">
@@ -18793,7 +18797,7 @@
         <v>8</v>
       </c>
       <c r="K469" s="8">
-        <f>MODE(A469:J469)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L469" s="16">
@@ -18832,7 +18836,7 @@
         <v>2</v>
       </c>
       <c r="K470" s="8">
-        <f>MODE(A470:J470)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="L470" s="16">
@@ -18871,7 +18875,7 @@
         <v>7</v>
       </c>
       <c r="K471" s="8">
-        <f>MODE(A471:J471)</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="L471" s="16">
@@ -18910,7 +18914,7 @@
         <v>5</v>
       </c>
       <c r="K472" s="8">
-        <f>MODE(A472:J472)</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L472" s="16">
@@ -18949,7 +18953,7 @@
         <v>8</v>
       </c>
       <c r="K473" s="8">
-        <f>MODE(A473:J473)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L473" s="16">
@@ -18988,7 +18992,7 @@
         <v>9</v>
       </c>
       <c r="K474" s="8">
-        <f>MODE(A474:J474)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L474" s="16">
@@ -19027,7 +19031,7 @@
         <v>0</v>
       </c>
       <c r="K475" s="8">
-        <f>MODE(A475:J475)</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L475" s="16">
@@ -19066,7 +19070,7 @@
         <v>1</v>
       </c>
       <c r="K476" s="8">
-        <f>MODE(A476:J476)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L476" s="16">
@@ -19105,7 +19109,7 @@
         <v>8</v>
       </c>
       <c r="K477" s="8">
-        <f>MODE(A477:J477)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L477" s="16">
@@ -19144,7 +19148,7 @@
         <v>4</v>
       </c>
       <c r="K478" s="8">
-        <f>MODE(A478:J478)</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="L478" s="16">
@@ -19183,7 +19187,7 @@
         <v>1</v>
       </c>
       <c r="K479" s="8">
-        <f>MODE(A479:J479)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L479" s="16">
@@ -19222,7 +19226,7 @@
         <v>2</v>
       </c>
       <c r="K480" s="8">
-        <f>MODE(A480:J480)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="L480" s="16">
@@ -19261,7 +19265,7 @@
         <v>5</v>
       </c>
       <c r="K481" s="8">
-        <f>MODE(A481:J481)</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L481" s="16">
@@ -19300,7 +19304,7 @@
         <v>9</v>
       </c>
       <c r="K482" s="8">
-        <f>MODE(A482:J482)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L482" s="16">
@@ -19339,7 +19343,7 @@
         <v>1</v>
       </c>
       <c r="K483" s="8">
-        <f>MODE(A483:J483)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L483" s="16">
@@ -19378,7 +19382,7 @@
         <v>9</v>
       </c>
       <c r="K484" s="8">
-        <f>MODE(A484:J484)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L484" s="16">
@@ -19417,7 +19421,7 @@
         <v>7</v>
       </c>
       <c r="K485" s="8">
-        <f>MODE(A485:J485)</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="L485" s="16">
@@ -19456,7 +19460,7 @@
         <v>5</v>
       </c>
       <c r="K486" s="8">
-        <f>MODE(A486:J486)</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L486" s="16">
@@ -19495,7 +19499,7 @@
         <v>4</v>
       </c>
       <c r="K487" s="8">
-        <f>MODE(A487:J487)</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="L487" s="16">
@@ -19534,7 +19538,7 @@
         <v>0</v>
       </c>
       <c r="K488" s="8">
-        <f>MODE(A488:J488)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L488" s="16">
@@ -19573,7 +19577,7 @@
         <v>8</v>
       </c>
       <c r="K489" s="8">
-        <f>MODE(A489:J489)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L489" s="16">
@@ -19612,7 +19616,7 @@
         <v>9</v>
       </c>
       <c r="K490" s="8">
-        <f>MODE(A490:J490)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L490" s="16">
@@ -19651,7 +19655,7 @@
         <v>9</v>
       </c>
       <c r="K491" s="8">
-        <f>MODE(A491:J491)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L491" s="16">
@@ -19690,7 +19694,7 @@
         <v>1</v>
       </c>
       <c r="K492" s="8">
-        <f>MODE(A492:J492)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="L492" s="16">
@@ -19729,7 +19733,7 @@
         <v>4</v>
       </c>
       <c r="K493" s="8">
-        <f>MODE(A493:J493)</f>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="L493" s="16">
@@ -19768,7 +19772,7 @@
         <v>5</v>
       </c>
       <c r="K494" s="8">
-        <f>MODE(A494:J494)</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="L494" s="16">
@@ -19807,7 +19811,7 @@
         <v>2</v>
       </c>
       <c r="K495" s="8">
-        <f>MODE(A495:J495)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="L495" s="16">
@@ -19846,7 +19850,7 @@
         <v>3</v>
       </c>
       <c r="K496" s="8">
-        <f>MODE(A496:J496)</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="L496" s="16">
@@ -19885,7 +19889,7 @@
         <v>7</v>
       </c>
       <c r="K497" s="8">
-        <f>MODE(A497:J497)</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="L497" s="16">
@@ -19924,7 +19928,7 @@
         <v>8</v>
       </c>
       <c r="K498" s="8">
-        <f>MODE(A498:J498)</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="L498" s="16">
@@ -19963,7 +19967,7 @@
         <v>9</v>
       </c>
       <c r="K499" s="8">
-        <f>MODE(A499:J499)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L499" s="16">
@@ -20002,7 +20006,7 @@
         <v>9</v>
       </c>
       <c r="K500" s="8">
-        <f>MODE(A500:J500)</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="L500" s="16">
@@ -20041,7 +20045,7 @@
         <v>0</v>
       </c>
       <c r="K501" s="8">
-        <f>MODE(A501:J501)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L501" s="16">
@@ -20080,7 +20084,7 @@
         <v>6</v>
       </c>
       <c r="K502" s="8">
-        <f>MODE(A502:J502)</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="L502" s="16">

</xml_diff>